<commit_message>
Found a problem with data import. Pushing before working on it
</commit_message>
<xml_diff>
--- a/server/beachData/Ontario_Beaches_Sample_List.xlsx
+++ b/server/beachData/Ontario_Beaches_Sample_List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
   <si>
     <t>BeachID</t>
   </si>
@@ -92,7 +92,7 @@
     <t>Whitby Beach</t>
   </si>
   <si>
-    <t>Port Glasgow </t>
+    <t>Port Glasgow</t>
   </si>
   <si>
     <t>Elgin</t>
@@ -152,13 +152,16 @@
     <t>Hillman</t>
   </si>
   <si>
-    <t>NEW BEACH THAT I CREATED </t>
+    <t>NEW BEACH THAT I CREATED</t>
   </si>
   <si>
     <t>WHATEVER</t>
   </si>
   <si>
     <t>NOT ONTARIO</t>
+  </si>
+  <si>
+    <t>BAWS</t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B38" activeCellId="0" pane="topLeft" sqref="B38"/>
+      <selection activeCell="F37" activeCellId="0" pane="topLeft" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1091,6 +1094,26 @@
         <v>2</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Admin beach creating/editing/removing/importing. Also fixed bug in beach import.
</commit_message>
<xml_diff>
--- a/server/beachData/Ontario_Beaches_Sample_List.xlsx
+++ b/server/beachData/Ontario_Beaches_Sample_List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
   <si>
     <t>BeachID</t>
   </si>
@@ -162,6 +162,39 @@
   </si>
   <si>
     <t>BAWS</t>
+  </si>
+  <si>
+    <t>wdjiasioj</t>
+  </si>
+  <si>
+    <t>dsads</t>
+  </si>
+  <si>
+    <t>zfd</t>
+  </si>
+  <si>
+    <t>EFS</t>
+  </si>
+  <si>
+    <t>2DASD</t>
+  </si>
+  <si>
+    <t>DSADSA</t>
+  </si>
+  <si>
+    <t>dsadas</t>
+  </si>
+  <si>
+    <t>adsas</t>
+  </si>
+  <si>
+    <t>feaf</t>
+  </si>
+  <si>
+    <t>fds</t>
+  </si>
+  <si>
+    <t>fsdfd</t>
   </si>
 </sst>
 </file>
@@ -357,10 +390,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F37" activeCellId="0" pane="topLeft" sqref="F37"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A23" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F41" activeCellId="0" pane="topLeft" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1114,6 +1147,86 @@
         <v>3</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
+      <c r="A39" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="40">
+      <c r="A40" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>2342</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="41">
+      <c r="A41" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>